<commit_message>
Added and updated docs
</commit_message>
<xml_diff>
--- a/Group project/Project Info/Project Task 1/Timeline/CMPG315_GROUP_DATES.xlsx
+++ b/Group project/Project Info/Project Task 1/Timeline/CMPG315_GROUP_DATES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b9e215ce13e2448/Desktop/NWU/NWU 2024/Modules/Semester 1/CMPG 315/Group project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMPG315_Group04_Files\CMPG315_GROUP04\Group project\Project Info\Project Task 1\Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83DA434-8BAD-4774-9679-A5CF57E29223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B66CD5C-B63D-4491-ACB1-61680F89D4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5772B818-03FF-422F-8D6F-A22D067566A7}"/>
   </bookViews>
@@ -233,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -333,11 +333,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -392,6 +409,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396E95B8-7E52-474D-8EDC-F05DC43F5E2A}">
   <dimension ref="B1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,11 +932,11 @@
       <c r="C10" s="17">
         <v>25</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="17">
         <v>1</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="18">
         <v>8</v>
       </c>
@@ -946,11 +969,11 @@
       <c r="C11" s="17">
         <v>26</v>
       </c>
-      <c r="D11" s="20"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="17">
         <v>2</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="17">
         <v>9</v>
       </c>
@@ -983,11 +1006,11 @@
       <c r="C12" s="17">
         <v>27</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="17">
         <v>3</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="17">
         <v>10</v>
       </c>
@@ -1020,11 +1043,11 @@
       <c r="C13" s="17">
         <v>28</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="17">
         <v>4</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="17">
         <v>11</v>
       </c>
@@ -1057,11 +1080,11 @@
       <c r="C14" s="26">
         <v>29</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="25">
         <v>5</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="34"/>
       <c r="G14" s="25">
         <v>12</v>
       </c>
@@ -1094,11 +1117,11 @@
       <c r="C15" s="17">
         <v>30</v>
       </c>
-      <c r="D15" s="24"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="17">
         <v>6</v>
       </c>
-      <c r="F15" s="24"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="17">
         <v>13</v>
       </c>
@@ -1131,11 +1154,11 @@
       <c r="C16" s="17">
         <v>31</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="17">
         <v>7</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="17">
         <v>14</v>
       </c>

</xml_diff>